<commit_message>
added cmsc tt chart
</commit_message>
<xml_diff>
--- a/by_year.xlsx
+++ b/by_year.xlsx
@@ -1,13 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="17240" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="17240" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="by_year.tsv" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
@@ -589,11 +591,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2088979208"/>
-        <c:axId val="-2088976120"/>
+        <c:axId val="-2085984840"/>
+        <c:axId val="-2084494968"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2088979208"/>
+        <c:axId val="-2085984840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -622,7 +624,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2088976120"/>
+        <c:crossAx val="-2084494968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -630,7 +632,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2088976120"/>
+        <c:axId val="-2084494968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -641,7 +643,266 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2088979208"/>
+        <c:crossAx val="-2085984840"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2400"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2400"/>
+              <a:t>CMSC Tenure-Track</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="2400" baseline="0"/>
+              <a:t> Faculty</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="2400"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.0545873822628359"/>
+          <c:y val="0.0893682588597843"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>by_year.tsv!$M$1:$AF$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1994.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1995.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1996.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1997.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1998.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1999.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2001.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2002.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2003.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2004.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2005.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2006.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2007.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2008.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2009.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2010.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2011.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2012.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2013.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>by_year.tsv!$M$2:$AF$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="-2085211608"/>
+        <c:axId val="2140242440"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2085211608"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2140242440"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2140242440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2085211608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -667,21 +928,60 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>50800</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>279400</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1022,8 +1322,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B8" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2:AF2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1332,6 +1632,41 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
   <extLst>

</xml_diff>

<commit_message>
ece => ee or ce
</commit_message>
<xml_diff>
--- a/by_year.xlsx
+++ b/by_year.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="17240" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="-36040" yWindow="-16900" windowWidth="25600" windowHeight="17560" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="by_year.tsv" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>year</t>
   </si>
@@ -29,7 +29,10 @@
     <t>CS</t>
   </si>
   <si>
-    <t>ECE</t>
+    <t>CE</t>
+  </si>
+  <si>
+    <t>EE</t>
   </si>
 </sst>
 </file>
@@ -97,17 +100,17 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="4000"/>
+              <a:defRPr sz="2400"/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="4000"/>
-              <a:t>CSEE Tenure</a:t>
+              <a:rPr lang="en-US" sz="2400"/>
+              <a:t>CSEE</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" sz="4000" baseline="0"/>
-              <a:t> Track Lines</a:t>
+              <a:rPr lang="en-US" sz="2400" baseline="0"/>
+              <a:t> TT faculty: EE, CS, CE</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US" sz="4000"/>
+            <a:endParaRPr lang="en-US" sz="2400"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -115,8 +118,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0406574579878838"/>
-          <c:y val="0.0403587443946188"/>
+          <c:x val="0.0772138247861168"/>
+          <c:y val="0.05420054200542"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -309,46 +312,46 @@
                   <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
                   <c:v>18.0</c:v>
                 </c:pt>
-                <c:pt idx="19">
-                  <c:v>22.0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>22.0</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>22.0</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>22.0</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>22.0</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>21.0</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>21.0</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>21.0</c:v>
-                </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="29">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
                   <c:v>20.0</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>19.0</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>20.0</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>19.0</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>21.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -363,12 +366,77 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>ECE</c:v>
+                  <c:v>CE</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="8"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="9"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="10"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="11"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="12"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="13"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
           <c:cat>
             <c:numRef>
               <c:f>by_year.tsv!$B$1:$AG$1</c:f>
@@ -490,6 +558,253 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>6.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>by_year.tsv!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>EE</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>by_year.tsv!$B$1:$AG$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>1983.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1984.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1985.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1986.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1987.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1988.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1989.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1990.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1991.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1992.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1993.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1994.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1995.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1996.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1997.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1998.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1999.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2001.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2002.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2003.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2004.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2005.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2006.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2007.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2008.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2009.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2010.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2011.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2012.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2013.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2014.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>by_year.tsv!$B$4:$AG$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
@@ -523,65 +838,64 @@
                   <c:v>9.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>11.0</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="21">
                   <c:v>11.0</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="22">
                   <c:v>11.0</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="23">
                   <c:v>11.0</c:v>
                 </c:pt>
-                <c:pt idx="18">
-                  <c:v>12.0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>12.0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>13.0</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>14.0</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>14.0</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>13.0</c:v>
-                </c:pt>
                 <c:pt idx="24">
-                  <c:v>13.0</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>12.0</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>12.0</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>14.0</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>15.0</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>14.0</c:v>
+                  <c:v>9.0</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>13.0</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>14.0</c:v>
+                  <c:v>9.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="inEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
           <c:showCatName val="0"/>
@@ -591,39 +905,21 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2069348040"/>
-        <c:axId val="-2069330040"/>
+        <c:axId val="-2122186856"/>
+        <c:axId val="-2122188216"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2069348040"/>
+        <c:axId val="-2122186856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1800"/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1800"/>
-                  <a:t>year</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2069330040"/>
+        <c:crossAx val="-2122188216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -631,24 +927,25 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2069330040"/>
+        <c:axId val="-2122188216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:minorGridlines/>
+        <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2069348040"/>
+        <c:crossAx val="-2122186856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -684,17 +981,17 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="2400"/>
+              <a:defRPr sz="2800"/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="2400"/>
-              <a:t>CMSC Tenure-Track</a:t>
+              <a:rPr lang="en-US" sz="2800"/>
+              <a:t>CMSC</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" sz="2400" baseline="0"/>
-              <a:t> Faculty</a:t>
+              <a:rPr lang="en-US" sz="2800" baseline="0"/>
+              <a:t> TT faculty 1994-2014</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US" sz="2400"/>
+            <a:endParaRPr lang="en-US" sz="2800"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -702,8 +999,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0545873822628359"/>
-          <c:y val="0.0893682588597843"/>
+          <c:x val="0.0394773833461748"/>
+          <c:y val="0.0465686274509804"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -721,10 +1018,10 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>by_year.tsv!$M$1:$AF$1</c:f>
+              <c:f>by_year.tsv!$M$1:$AG$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>1994.0</c:v>
                 </c:pt>
@@ -784,16 +1081,19 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>2013.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2014.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>by_year.tsv!$M$2:$AF$2</c:f>
+              <c:f>by_year.tsv!$M$2:$AG$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>16.0</c:v>
                 </c:pt>
@@ -816,43 +1116,46 @@
                   <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>18.0</c:v>
                 </c:pt>
-                <c:pt idx="8">
-                  <c:v>22.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>22.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>22.0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>22.0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>22.0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>21.0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>21.0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>21.0</c:v>
-                </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="18">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>20.0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>19.0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>20.0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>19.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -867,11 +1170,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2143217784"/>
-        <c:axId val="-2143214808"/>
+        <c:axId val="2127368808"/>
+        <c:axId val="-2120972856"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2143217784"/>
+        <c:axId val="2127368808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -881,7 +1184,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2143214808"/>
+        <c:crossAx val="-2120972856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -889,7 +1192,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2143214808"/>
+        <c:axId val="-2120972856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -900,7 +1203,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2143217784"/>
+        <c:crossAx val="2127368808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -921,16 +1224,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>698500</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -958,16 +1261,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>406400</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>749300</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>146050</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>660400</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1313,10 +1616,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG3"/>
+  <dimension ref="A1:AG4"/>
   <sheetViews>
     <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:AF2"/>
+      <selection activeCell="M2" sqref="M2:AG2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1481,46 +1784,46 @@
         <v>16</v>
       </c>
       <c r="T2">
+        <v>17</v>
+      </c>
+      <c r="U2">
+        <v>21</v>
+      </c>
+      <c r="V2">
+        <v>21</v>
+      </c>
+      <c r="W2">
+        <v>21</v>
+      </c>
+      <c r="X2">
+        <v>21</v>
+      </c>
+      <c r="Y2">
+        <v>21</v>
+      </c>
+      <c r="Z2">
+        <v>20</v>
+      </c>
+      <c r="AA2">
+        <v>20</v>
+      </c>
+      <c r="AB2">
+        <v>20</v>
+      </c>
+      <c r="AC2">
+        <v>19</v>
+      </c>
+      <c r="AD2">
         <v>18</v>
       </c>
-      <c r="U2">
-        <v>22</v>
-      </c>
-      <c r="V2">
-        <v>22</v>
-      </c>
-      <c r="W2">
-        <v>22</v>
-      </c>
-      <c r="X2">
-        <v>22</v>
-      </c>
-      <c r="Y2">
-        <v>22</v>
-      </c>
-      <c r="Z2">
-        <v>21</v>
-      </c>
-      <c r="AA2">
-        <v>21</v>
-      </c>
-      <c r="AB2">
-        <v>21</v>
-      </c>
-      <c r="AC2">
+      <c r="AE2">
+        <v>19</v>
+      </c>
+      <c r="AF2">
+        <v>18</v>
+      </c>
+      <c r="AG2">
         <v>20</v>
-      </c>
-      <c r="AD2">
-        <v>19</v>
-      </c>
-      <c r="AE2">
-        <v>20</v>
-      </c>
-      <c r="AF2">
-        <v>19</v>
-      </c>
-      <c r="AG2">
-        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:33">
@@ -1537,91 +1840,192 @@
         <v>0</v>
       </c>
       <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
         <v>1</v>
       </c>
-      <c r="F3">
+      <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="S3">
+        <v>2</v>
+      </c>
+      <c r="T3">
         <v>3</v>
       </c>
-      <c r="G3">
+      <c r="U3">
+        <v>3</v>
+      </c>
+      <c r="V3">
+        <v>3</v>
+      </c>
+      <c r="W3">
+        <v>4</v>
+      </c>
+      <c r="X3">
+        <v>4</v>
+      </c>
+      <c r="Y3">
+        <v>3</v>
+      </c>
+      <c r="Z3">
+        <v>3</v>
+      </c>
+      <c r="AA3">
+        <v>3</v>
+      </c>
+      <c r="AB3">
+        <v>3</v>
+      </c>
+      <c r="AC3">
         <v>5</v>
       </c>
-      <c r="H3">
+      <c r="AD3">
         <v>6</v>
       </c>
-      <c r="I3">
+      <c r="AE3">
         <v>6</v>
       </c>
-      <c r="J3">
+      <c r="AF3">
+        <v>6</v>
+      </c>
+      <c r="AG3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <v>5</v>
+      </c>
+      <c r="H4">
+        <v>6</v>
+      </c>
+      <c r="I4">
+        <v>6</v>
+      </c>
+      <c r="J4">
         <v>8</v>
       </c>
-      <c r="K3">
+      <c r="K4">
         <v>9</v>
       </c>
-      <c r="L3">
+      <c r="L4">
         <v>9</v>
       </c>
-      <c r="M3">
+      <c r="M4">
         <v>9</v>
       </c>
-      <c r="N3">
+      <c r="N4">
         <v>9</v>
       </c>
-      <c r="O3">
+      <c r="O4">
         <v>9</v>
       </c>
-      <c r="P3">
+      <c r="P4">
+        <v>10</v>
+      </c>
+      <c r="Q4">
+        <v>10</v>
+      </c>
+      <c r="R4">
+        <v>10</v>
+      </c>
+      <c r="S4">
+        <v>9</v>
+      </c>
+      <c r="T4">
+        <v>10</v>
+      </c>
+      <c r="U4">
+        <v>10</v>
+      </c>
+      <c r="V4">
         <v>11</v>
       </c>
-      <c r="Q3">
+      <c r="W4">
         <v>11</v>
       </c>
-      <c r="R3">
+      <c r="X4">
         <v>11</v>
       </c>
-      <c r="S3">
+      <c r="Y4">
         <v>11</v>
       </c>
-      <c r="T3">
-        <v>12</v>
-      </c>
-      <c r="U3">
-        <v>12</v>
-      </c>
-      <c r="V3">
-        <v>13</v>
-      </c>
-      <c r="W3">
-        <v>14</v>
-      </c>
-      <c r="X3">
-        <v>14</v>
-      </c>
-      <c r="Y3">
-        <v>13</v>
-      </c>
-      <c r="Z3">
-        <v>13</v>
-      </c>
-      <c r="AA3">
-        <v>12</v>
-      </c>
-      <c r="AB3">
-        <v>12</v>
-      </c>
-      <c r="AC3">
-        <v>14</v>
-      </c>
-      <c r="AD3">
-        <v>15</v>
-      </c>
-      <c r="AE3">
-        <v>14</v>
-      </c>
-      <c r="AF3">
-        <v>13</v>
-      </c>
-      <c r="AG3">
-        <v>14</v>
+      <c r="Z4">
+        <v>11</v>
+      </c>
+      <c r="AA4">
+        <v>10</v>
+      </c>
+      <c r="AB4">
+        <v>10</v>
+      </c>
+      <c r="AC4">
+        <v>10</v>
+      </c>
+      <c r="AD4">
+        <v>10</v>
+      </c>
+      <c r="AE4">
+        <v>9</v>
+      </c>
+      <c r="AF4">
+        <v>8</v>
+      </c>
+      <c r="AG4">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1638,7 +2042,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData/>
@@ -1656,7 +2062,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData/>

</xml_diff>